<commit_message>
update code of AOS project selenium
</commit_message>
<xml_diff>
--- a/selen_projectAOS/Tests_AOS.xlsx
+++ b/selen_projectAOS/Tests_AOS.xlsx
@@ -1109,6 +1109,36 @@
           <t>Test Result</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>